<commit_message>
V2 de la carte sur Altium
A montrer à PEB!
</commit_message>
<xml_diff>
--- a/Composant Carte emulateur AX12.xlsx
+++ b/Composant Carte emulateur AX12.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Connecteur Molex AX12</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Pic 30F2010-30I/SO</t>
   </si>
   <si>
-    <t>74LVC2G241 (Porte 3 états)</t>
-  </si>
-  <si>
     <t>10µF</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Choix 2</t>
   </si>
   <si>
-    <t>Il Faudra pour ce choix avoir 2 GPIO pour le drive de la porte</t>
-  </si>
-  <si>
     <t>Déjà acheter</t>
   </si>
   <si>
@@ -94,15 +88,9 @@
     <t>Quantité min</t>
   </si>
   <si>
-    <t>1µF (choix 1)</t>
-  </si>
-  <si>
     <t>http://www.rs-particuliers.com/WebCatalog/Condensateur_ceramique_multicouche__Kemet_C0805C106K4PACTU__10%C2%B5F__16_V_cc__dielectrique_X5R__boitier_0805-6911161.aspx</t>
   </si>
   <si>
-    <t>Clock 4 MHz</t>
-  </si>
-  <si>
     <t>? Ou on l'achete</t>
   </si>
   <si>
@@ -127,10 +115,100 @@
     <t>http://www.rs-particuliers.com/WebCatalog/Microcontr%C3%B4leur__16bit__dsPIC__12_kB__1_024_B_Flash__30MIPS__28_SOIC-6668245.aspx</t>
   </si>
   <si>
-    <t>SN74AHC1G126DCKR (Porte 3 états)</t>
-  </si>
-  <si>
     <t>http://www.rs-particuliers.com/WebCatalog/Buffer_de_bus__AHC__SN74AHC1G126DCKR__115_ns@_33_V__8mA_SC_70_5_broches_2__5_5_V-6518074.aspx</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>2,15*2,4*1,1</t>
+  </si>
+  <si>
+    <t>74LVC2G241 - VSSOP (Porte 3 états)</t>
+  </si>
+  <si>
+    <t>Choix 3</t>
+  </si>
+  <si>
+    <t>3,05*1,75*1,3</t>
+  </si>
+  <si>
+    <t>SN74AHC1G126DBVR - SOT-23</t>
+  </si>
+  <si>
+    <t>http://www.rs-particuliers.com/WebCatalog/Buffer_de_bus__AHC__SN74AHC1G126DBVR__85_ns@_50_pF__8mA_SOT_23_5_broches_2__5_5_V-8099449.aspx</t>
+  </si>
+  <si>
+    <t>Il Faudra pour ce choix avoir 2 GPIO</t>
+  </si>
+  <si>
+    <t>TC7WH240FU - SSOP</t>
+  </si>
+  <si>
+    <t>Choix 4</t>
+  </si>
+  <si>
+    <t>2,9*2,8*1,1</t>
+  </si>
+  <si>
+    <t>http://www.rs-particuliers.com/WebCatalog/Double_buffer_de_bus__CMOS__TC7WH240FUTE12L_F__15_ns@_15_pF__8mA_SSOP_8_broches_2__5_5_V-8912841.aspx</t>
+  </si>
+  <si>
+    <t>2,1*2,4*1,1</t>
+  </si>
+  <si>
+    <t>Choix 5</t>
+  </si>
+  <si>
+    <t>SN74AHC1G125DVBR - SOT-23</t>
+  </si>
+  <si>
+    <t>2,9*1,6*1,15</t>
+  </si>
+  <si>
+    <t>http://www.rs-particuliers.com/WebCatalog/Buffer_de_bus__AHC__SN74AHC1G125DBVR__115_ns@_33_V__8mA_SOT_23_5_broches_2__5_5_V-528280.aspx</t>
+  </si>
+  <si>
+    <t>1µF</t>
+  </si>
+  <si>
+    <t>SN74AHC1G126DCKR - SC-70</t>
+  </si>
+  <si>
+    <t>Clock 4 MHz - IQXO-70</t>
+  </si>
+  <si>
+    <t>Angle droit</t>
+  </si>
+  <si>
+    <t>Pas de 2,54mm</t>
+  </si>
+  <si>
+    <t>Droit</t>
+  </si>
+  <si>
+    <t>http://www.rs-particuliers.com/WebCatalog/Connecteur_Male__Traversant__2_Contacts__1_rangee__Droit__au_pas_de_254mm-7020161.aspx</t>
+  </si>
+  <si>
+    <t>http://www.rs-particuliers.com/WebCatalog/Connecteur_Male__Traversant__6_Contacts__1_rangee__Angle_droit__au_pas_de_254mm-7019783.aspx</t>
+  </si>
+  <si>
+    <t>http://www.rs-particuliers.com/WebCatalog/Connecteur_Male__Traversant__2_Contacts__1_rangee__Angle_droit__au_pas_de_254mm-7019773.aspx</t>
+  </si>
+  <si>
+    <t>http://www.rs-particuliers.com/WebCatalog/Connecteur_Male__Traversant__3_Contacts__1_rangee__Angle_droit__au_pas_de_254mm-7019777.aspx</t>
+  </si>
+  <si>
+    <t>6,5*3,56*1,6</t>
+  </si>
+  <si>
+    <t>nb de broches</t>
+  </si>
+  <si>
+    <t>Restant</t>
+  </si>
+  <si>
+    <t>Prix</t>
   </si>
 </sst>
 </file>
@@ -154,15 +232,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -170,14 +254,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -483,23 +661,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="12" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -510,19 +690,28 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -530,252 +719,627 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0.24</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1.2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4">
+        <f>E4-C4</f>
+        <v>3</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.88</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1.78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L22" si="0">E5-C5</f>
+        <v>-1</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.33</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1.65</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.59</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>2.95</v>
+      </c>
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <v>1.1599999999999999</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="E11" s="3">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="3">
+        <v>8</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="4"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="E12" s="6">
+        <v>50</v>
+      </c>
+      <c r="F12" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="13">
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="8"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.31</v>
+      </c>
+      <c r="E13" s="15">
+        <v>15</v>
+      </c>
+      <c r="F13" s="15">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="13">
+        <v>5</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="8"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="E14" s="6">
+        <v>25</v>
+      </c>
+      <c r="F14" s="6">
+        <v>7.75</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="13">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="8"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.34</v>
+      </c>
+      <c r="E15" s="10">
+        <v>10</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="10">
+        <v>8</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="12"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0.03</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>1.5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>0.17</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>1.7</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.08</v>
+      </c>
+      <c r="E18">
+        <v>50</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="L22">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0.48</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>4.8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>0.05</v>
-      </c>
-      <c r="E11">
-        <v>50</v>
-      </c>
-      <c r="F11">
-        <v>2.5</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0.03</v>
-      </c>
-      <c r="E12">
-        <v>50</v>
-      </c>
-      <c r="F12">
-        <v>1.5</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>0.17</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>1.7</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>0.08</v>
-      </c>
-      <c r="E14">
-        <v>50</v>
-      </c>
-      <c r="F14">
-        <v>4</v>
-      </c>
-      <c r="J14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="G18" t="s">
-        <v>33</v>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25">
+        <f>SUM(F16:F22,F13,F4:F10)</f>
+        <v>25.490000000000002</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J9" r:id="rId1"/>
-    <hyperlink ref="J11" r:id="rId2"/>
-    <hyperlink ref="J13" r:id="rId3"/>
-    <hyperlink ref="J12" r:id="rId4"/>
+    <hyperlink ref="M10" r:id="rId1"/>
+    <hyperlink ref="M12" r:id="rId2"/>
+    <hyperlink ref="M17" r:id="rId3"/>
+    <hyperlink ref="M16" r:id="rId4"/>
+    <hyperlink ref="M13" r:id="rId5"/>
+    <hyperlink ref="M5" r:id="rId6"/>
+    <hyperlink ref="M6" r:id="rId7"/>
+    <hyperlink ref="M7" r:id="rId8"/>
+    <hyperlink ref="M4" r:id="rId9"/>
+    <hyperlink ref="M18" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modif Altium + Code
V2 du PCB avec nouvelle porte 3 états.
Epuration du code en rajoutant beaucoup de define
</commit_message>
<xml_diff>
--- a/Composant Carte emulateur AX12.xlsx
+++ b/Composant Carte emulateur AX12.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
   <si>
     <t>Connecteur Molex AX12</t>
   </si>
@@ -52,12 +52,6 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>330o</t>
-  </si>
-  <si>
     <t>Condo cms 0805</t>
   </si>
   <si>
@@ -209,6 +203,15 @@
   </si>
   <si>
     <t>Prix</t>
+  </si>
+  <si>
+    <t>Prix d'1 carte</t>
+  </si>
+  <si>
+    <t>Prix min</t>
+  </si>
+  <si>
+    <t>150o</t>
   </si>
 </sst>
 </file>
@@ -661,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC25"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,13 +676,13 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="0.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="12" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="13" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -690,44 +693,47 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="L1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -741,23 +747,27 @@
       <c r="F4">
         <v>1.2</v>
       </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4">
+      <c r="G4">
+        <f>D4*C4</f>
+        <v>0.48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4">
         <f>E4-C4</f>
         <v>3</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="N4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -771,23 +781,27 @@
       <c r="F5">
         <v>1.78</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <f t="shared" ref="G5:G21" si="0">D5*C5</f>
+        <v>1.76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M21" si="1">E5-C5</f>
+        <v>-1</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L22" si="0">E5-C5</f>
-        <v>-1</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -801,23 +815,27 @@
       <c r="F6">
         <v>1.65</v>
       </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="N6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -831,18 +849,22 @@
       <c r="F7">
         <v>2.95</v>
       </c>
-      <c r="G7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="N7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -858,39 +880,47 @@
       <c r="F8">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8">
         <v>4</v>
       </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
+      <c r="M8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9">
         <v>4</v>
       </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
+      <c r="M9">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -906,20 +936,24 @@
       <c r="F10">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="N10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -933,22 +967,25 @@
       <c r="F11" s="3">
         <v>4.8</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="3"/>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="3">
         <v>8</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="0"/>
+      <c r="M11">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -964,14 +1001,15 @@
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
-      <c r="AC11" s="4"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="4"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
@@ -985,25 +1023,28 @@
       <c r="F12" s="6">
         <v>2.5</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="6"/>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="13">
+      <c r="J12" s="6"/>
+      <c r="K12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="13">
         <v>5</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
+      <c r="M12">
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="M12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="6"/>
+      <c r="N12" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -1018,14 +1059,15 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
-      <c r="AC12" s="8"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="8"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="15">
         <v>2</v>
@@ -1039,25 +1081,28 @@
       <c r="F13" s="15">
         <v>4.6500000000000004</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="6"/>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="N13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="13">
-        <v>5</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -1072,14 +1117,15 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
-      <c r="AC13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="8"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
@@ -1093,23 +1139,26 @@
       <c r="F14" s="6">
         <v>7.75</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K14" s="13">
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="13">
         <v>5</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="0"/>
+      <c r="M14">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="M14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="N14" s="6"/>
+      <c r="N14" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
@@ -1124,14 +1173,15 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
-      <c r="AC14" s="8"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="8"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="10">
         <v>1</v>
@@ -1145,23 +1195,26 @@
       <c r="F15" s="10">
         <v>3.4</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K15" s="10">
+      <c r="J15" s="10"/>
+      <c r="K15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="10">
         <v>8</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
+      <c r="M15">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="M15" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N15" s="10"/>
+      <c r="N15" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
@@ -1176,14 +1229,15 @@
       <c r="Z15" s="10"/>
       <c r="AA15" s="10"/>
       <c r="AB15" s="10"/>
-      <c r="AC15" s="12"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="12"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1197,15 +1251,19 @@
       <c r="F16">
         <v>1.5</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="0"/>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -1221,15 +1279,19 @@
       <c r="F17">
         <v>1.7</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1245,101 +1307,117 @@
       <c r="F18">
         <v>4</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.91639999999999999</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>9.1639999999999997</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0.91639999999999999</v>
+      </c>
+      <c r="H21" t="s">
         <v>27</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>26</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="G22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="0"/>
+      <c r="M21">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24">
+        <f>SUM(F16:F21,F13,F4:F10)</f>
+        <v>34.654000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25">
-        <f>SUM(F16:F22,F13,F4:F10)</f>
-        <v>25.490000000000002</v>
+        <f>SUM(G4:G10,G13,G16:G21)</f>
+        <v>11.206399999999999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M10" r:id="rId1"/>
-    <hyperlink ref="M12" r:id="rId2"/>
-    <hyperlink ref="M17" r:id="rId3"/>
-    <hyperlink ref="M16" r:id="rId4"/>
-    <hyperlink ref="M13" r:id="rId5"/>
-    <hyperlink ref="M5" r:id="rId6"/>
-    <hyperlink ref="M6" r:id="rId7"/>
-    <hyperlink ref="M7" r:id="rId8"/>
-    <hyperlink ref="M4" r:id="rId9"/>
-    <hyperlink ref="M18" r:id="rId10"/>
+    <hyperlink ref="N10" r:id="rId1"/>
+    <hyperlink ref="N12" r:id="rId2"/>
+    <hyperlink ref="N17" r:id="rId3"/>
+    <hyperlink ref="N16" r:id="rId4"/>
+    <hyperlink ref="N13" r:id="rId5"/>
+    <hyperlink ref="N5" r:id="rId6"/>
+    <hyperlink ref="N6" r:id="rId7"/>
+    <hyperlink ref="N7" r:id="rId8"/>
+    <hyperlink ref="N4" r:id="rId9"/>
+    <hyperlink ref="N18" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modif composant à acheter
</commit_message>
<xml_diff>
--- a/Composant Carte emulateur AX12.xlsx
+++ b/Composant Carte emulateur AX12.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>Connecteur Molex AX12</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Resistance cms 0805</t>
   </si>
   <si>
-    <t>? Ou on les achetes</t>
-  </si>
-  <si>
     <t>Choix 1</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>http://www.rs-particuliers.com/WebCatalog/Condensateur_ceramique_multicouche__Kemet_C0805C106K4PACTU__10%C2%B5F__16_V_cc__dielectrique_X5R__boitier_0805-6911161.aspx</t>
   </si>
   <si>
-    <t>? Ou on l'achete</t>
-  </si>
-  <si>
     <t>Déjà acheté</t>
   </si>
   <si>
@@ -212,6 +206,15 @@
   </si>
   <si>
     <t>150o</t>
+  </si>
+  <si>
+    <t>Déjà au local</t>
+  </si>
+  <si>
+    <t>http://www.rs-particuliers.com/WebCatalog/Oscillateur_a_quartz__4_MHz__%C2%B125ppm_HCMOS__15pF__CMS__7_x_5_x_14mm__4_broches-6720814.aspx</t>
+  </si>
+  <si>
+    <t>7*5*1,4</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
   <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,28 +696,28 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -725,7 +728,7 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -733,7 +736,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -752,14 +755,14 @@
         <v>0.48</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M4">
         <f>E4-C4</f>
         <v>3</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -767,7 +770,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -786,14 +789,14 @@
         <v>1.76</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M5">
         <f t="shared" ref="M5:M21" si="1">E5-C5</f>
         <v>-1</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -801,7 +804,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -820,14 +823,14 @@
         <v>0.33</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -835,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -854,14 +857,14 @@
         <v>0.59</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -885,10 +888,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -900,24 +903,36 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9">
+        <v>1.96</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1.96</v>
+      </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
+        <v>1.96</v>
+      </c>
+      <c r="K9" t="s">
+        <v>66</v>
       </c>
       <c r="L9">
         <v>4</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -945,15 +960,15 @@
         <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -972,12 +987,12 @@
         <v>0.48</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L11" s="3">
         <v>8</v>
@@ -1006,10 +1021,10 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
@@ -1028,12 +1043,12 @@
         <v>0.1</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L12" s="13">
         <v>5</v>
@@ -1043,7 +1058,7 @@
         <v>48</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
@@ -1064,10 +1079,10 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="15">
         <v>2</v>
@@ -1086,12 +1101,12 @@
         <v>0.62</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L13" s="13">
         <v>5</v>
@@ -1101,7 +1116,7 @@
         <v>13</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
@@ -1122,10 +1137,10 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
@@ -1147,7 +1162,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L14" s="13">
         <v>5</v>
@@ -1157,7 +1172,7 @@
         <v>23</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -1178,10 +1193,10 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="10">
         <v>1</v>
@@ -1203,7 +1218,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L15" s="10">
         <v>8</v>
@@ -1213,7 +1228,7 @@
         <v>9</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
@@ -1237,7 +1252,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1260,7 +1275,7 @@
         <v>49</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1288,7 +1303,7 @@
         <v>8</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1316,7 +1331,7 @@
         <v>49</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1324,7 +1339,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1334,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M19">
         <f t="shared" si="1"/>
@@ -1353,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
@@ -1362,7 +1377,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1381,7 +1396,7 @@
         <v>0.91639999999999999</v>
       </c>
       <c r="H21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M21">
         <f t="shared" si="1"/>
@@ -1390,20 +1405,20 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <f>SUM(F16:F21,F13,F4:F10)</f>
-        <v>34.654000000000003</v>
+        <v>36.614000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F25">
         <f>SUM(G4:G10,G13,G16:G21)</f>
-        <v>11.206399999999999</v>
+        <v>13.166399999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1418,6 +1433,7 @@
     <hyperlink ref="N7" r:id="rId8"/>
     <hyperlink ref="N4" r:id="rId9"/>
     <hyperlink ref="N18" r:id="rId10"/>
+    <hyperlink ref="N9" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modif valeurs resistances pour DDT et capteur de courant + Rajout sur liste composants
</commit_message>
<xml_diff>
--- a/Composant Carte emulateur AX12.xlsx
+++ b/Composant Carte emulateur AX12.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Connecteur Molex AX12</t>
   </si>
@@ -217,7 +217,25 @@
     <t>1K</t>
   </si>
   <si>
-    <t>63K</t>
+    <t>4K7</t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/resistances-cms/2230528/</t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/resistances-cms/8101892/</t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/resistances-cms/8280737/</t>
+  </si>
+  <si>
+    <t>750o   (choix 1)</t>
+  </si>
+  <si>
+    <t>750o   (choix 2)</t>
+  </si>
+  <si>
+    <t>COMME TU VEUX ça dépend du nombre que tu veux</t>
   </si>
 </sst>
 </file>
@@ -360,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -380,6 +398,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -685,16 +705,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AD30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="8" max="8" width="31.5703125" customWidth="1"/>
@@ -766,14 +786,14 @@
         <v>1.78</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G24" si="0">D4*C4</f>
+        <f t="shared" ref="G4:G26" si="0">D4*C4</f>
         <v>1.76</v>
       </c>
       <c r="H4" t="s">
         <v>47</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M24" si="1">E4-C4</f>
+        <f t="shared" ref="M4:M26" si="1">E4-C4</f>
         <v>-1</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -1332,49 +1352,81 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A19" s="6"/>
+      <c r="B19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>5</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="M19">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>4</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A20" s="6"/>
+      <c r="B20" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="E20" s="10">
+        <v>100</v>
+      </c>
+      <c r="F20" s="10">
+        <v>2</v>
+      </c>
+      <c r="G20" s="10">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="H20" s="20"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>99</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
@@ -1385,89 +1437,139 @@
       </c>
       <c r="M21">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>67</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="G22">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.01</v>
+      </c>
+      <c r="E23">
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <v>0.5</v>
+      </c>
+      <c r="G23">
+        <f>D23*C23</f>
+        <v>0.01</v>
+      </c>
+      <c r="H23" s="18"/>
+      <c r="M23">
+        <f>E23-C23</f>
+        <v>49</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="G24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="18"/>
-      <c r="M22">
+      <c r="H24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="G23">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="M23">
+      <c r="M25">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
         <v>0.91639999999999999</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <v>10</v>
       </c>
-      <c r="F24">
+      <c r="F26">
         <v>9.1639999999999997</v>
       </c>
-      <c r="G24">
+      <c r="G26">
         <f t="shared" si="0"/>
         <v>0.91639999999999999</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H26" t="s">
         <v>22</v>
       </c>
-      <c r="M24">
+      <c r="M26">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
         <v>54</v>
       </c>
-      <c r="F27">
-        <f>SUM(F15:F24,F12,F4:F9)</f>
-        <v>35.414000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
+      <c r="F29">
+        <f>SUM(F15:F26,F12,F4:F9)</f>
+        <v>38.913999999999994</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
         <v>55</v>
       </c>
-      <c r="F28">
-        <f>SUM(G4:G9,G12,G15:G24)</f>
-        <v>12.766399999999997</v>
+      <c r="F30">
+        <f>SUM(G4:G9,G12,G15:G26)</f>
+        <v>12.996399999999996</v>
       </c>
     </row>
   </sheetData>
@@ -1482,6 +1584,9 @@
     <hyperlink ref="N6" r:id="rId8"/>
     <hyperlink ref="N17" r:id="rId9"/>
     <hyperlink ref="N8" r:id="rId10"/>
+    <hyperlink ref="N23" r:id="rId11"/>
+    <hyperlink ref="N20" r:id="rId12"/>
+    <hyperlink ref="N19" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modif Capteur courant + liste composants
</commit_message>
<xml_diff>
--- a/Composant Carte emulateur AX12.xlsx
+++ b/Composant Carte emulateur AX12.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Connecteur Molex AX12</t>
   </si>
@@ -214,9 +214,6 @@
     <t>10K</t>
   </si>
   <si>
-    <t>1K</t>
-  </si>
-  <si>
     <t>4K7</t>
   </si>
   <si>
@@ -236,6 +233,12 @@
   </si>
   <si>
     <t>COMME TU VEUX ça dépend du nombre que tu veux</t>
+  </si>
+  <si>
+    <t>1o</t>
+  </si>
+  <si>
+    <t>http://fr.rs-online.com/web/p/resistances-cms/8711008/</t>
   </si>
 </sst>
 </file>
@@ -707,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1340,7 @@
         <v>57</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -1348,96 +1351,97 @@
       </c>
       <c r="M18">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E19" s="3">
-        <v>5</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="H19" s="19" t="s">
+      <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="18"/>
       <c r="M19">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>70</v>
+        <v>-1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>5</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="10">
-        <v>1</v>
-      </c>
-      <c r="D20" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="E20" s="10">
-        <v>100</v>
-      </c>
-      <c r="F20" s="10">
-        <v>2</v>
-      </c>
-      <c r="G20" s="10">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A21" s="6"/>
+      <c r="B21" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="10">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="E21" s="10">
+        <v>100</v>
+      </c>
+      <c r="F21" s="10">
+        <v>2</v>
+      </c>
+      <c r="G21" s="10">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="H21" s="20"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
       <c r="M21">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>99</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1461,7 +1465,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1479,13 +1483,15 @@
         <f>D23*C23</f>
         <v>0.01</v>
       </c>
-      <c r="H23" s="18"/>
+      <c r="H23" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="M23">
         <f>E23-C23</f>
         <v>49</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1585,8 +1591,8 @@
     <hyperlink ref="N17" r:id="rId9"/>
     <hyperlink ref="N8" r:id="rId10"/>
     <hyperlink ref="N23" r:id="rId11"/>
-    <hyperlink ref="N20" r:id="rId12"/>
-    <hyperlink ref="N19" r:id="rId13"/>
+    <hyperlink ref="N21" r:id="rId12"/>
+    <hyperlink ref="N20" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>